<commit_message>
Updates to library decoder - simplifiaction of Chem_ID to treatment, more universal for my scripts!
</commit_message>
<xml_diff>
--- a/CHEMdiv_rescreen_DJK.xlsx
+++ b/CHEMdiv_rescreen_DJK.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dankelpsch/Carnegie/People/Lishann Ingram/Final_folder/ChemDIV Secondary Screen-MummLabRobots /20220401_wk2_114plates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dankelpsch/Carnegie/Data/Screen/ChemDiv Library/Hit_rescreen/LMI_hit_rescreen/20220401_wk2_114plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE73D27-CECA-D642-9986-F2D61A1253B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F6C958-D2D3-1842-B08D-434156F96851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10300" yWindow="4720" windowWidth="23700" windowHeight="15720" xr2:uid="{848C83AE-DA71-A34C-B981-CBE322373055}"/>
   </bookViews>
@@ -652,10 +652,10 @@
     <t>Fish_addition_notes</t>
   </si>
   <si>
-    <t>Chem_ID</t>
-  </si>
-  <si>
     <t>ChemDiv_rescreen_plate</t>
+  </si>
+  <si>
+    <t>Treatment</t>
   </si>
 </sst>
 </file>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D254AE12-9178-8D49-8C10-79C5592488B1}">
   <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B35" sqref="B3:B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1096,7 +1096,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>201</v>
@@ -1111,7 +1111,7 @@
         <v>204</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>